<commit_message>
Actualizacion 2 a la base de datos de patrocinios
</commit_message>
<xml_diff>
--- a/Patrocinio/Base de datos patricinadores.xlsx
+++ b/Patrocinio/Base de datos patricinadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\entre\OneDrive\Desktop\FTC-Into_The_Deep\Patrocinio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F7867004-1E25-48C8-8B7C-F38EDBF2D99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF65441-5678-41D5-9B03-4DB43B9412B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BA4392A7-1F24-0648-8323-50C177A81C55}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="116">
   <si>
     <t xml:space="preserve">Juan Valdez </t>
   </si>
@@ -284,9 +284,6 @@
     <t>Bosi</t>
   </si>
   <si>
-    <t>LifeMIles</t>
-  </si>
-  <si>
     <t>Pepsi</t>
   </si>
   <si>
@@ -354,6 +351,39 @@
   </si>
   <si>
     <t>Unal</t>
+  </si>
+  <si>
+    <t>LifeMiles</t>
+  </si>
+  <si>
+    <t>Reebook</t>
+  </si>
+  <si>
+    <t>Ecopetrol</t>
+  </si>
+  <si>
+    <t>No están interesados</t>
+  </si>
+  <si>
+    <t>Respuesta automática</t>
+  </si>
+  <si>
+    <t>No reciben mensajes</t>
+  </si>
+  <si>
+    <t>Correo pendiente a: ANA.CELIS@ramo.com.co</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Correo pendiente a: dmorales@colombina.com </t>
+  </si>
+  <si>
+    <t>Hacer propuesta presencial</t>
+  </si>
+  <si>
+    <t>Correo pendiente a: smaya@wingo.com o mchaves@wingo.com</t>
+  </si>
+  <si>
+    <t>Esperando respuesta</t>
   </si>
 </sst>
 </file>
@@ -404,7 +434,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -415,6 +445,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -730,38 +763,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953E118B-2559-0648-84DD-D994D8679C8A}">
-  <dimension ref="A1:F96"/>
+  <dimension ref="A1:F98"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A107" sqref="A107"/>
+      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20.296875" customWidth="1"/>
-    <col min="3" max="3" width="17" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
+    <col min="5" max="5" width="25.09765625" style="2" customWidth="1"/>
+    <col min="6" max="6" width="58.69921875" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>94</v>
-      </c>
-      <c r="B1" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -772,10 +807,7 @@
         <v>0</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
@@ -786,10 +818,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -800,7 +838,13 @@
         <v>2</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -811,7 +855,13 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -822,10 +872,13 @@
         <v>4</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -836,7 +889,13 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -846,8 +905,14 @@
       <c r="B8" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="2" t="s">
-        <v>90</v>
+      <c r="D8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>111</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -858,10 +923,13 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -871,8 +939,14 @@
       <c r="B10" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="2" t="s">
-        <v>90</v>
+      <c r="D10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -883,7 +957,13 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E11" s="2" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -891,7 +971,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -902,10 +982,16 @@
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -916,10 +1002,13 @@
         <v>11</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -930,10 +1019,13 @@
         <v>12</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -944,13 +1036,19 @@
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -958,10 +1056,19 @@
         <v>14</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -969,13 +1076,13 @@
         <v>15</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D18" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -983,13 +1090,19 @@
         <v>16</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -997,13 +1110,13 @@
         <v>17</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1011,13 +1124,13 @@
         <v>18</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1025,13 +1138,13 @@
         <v>19</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1039,13 +1152,13 @@
         <v>20</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1053,10 +1166,10 @@
         <v>21</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1064,13 +1177,13 @@
         <v>22</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1078,13 +1191,13 @@
         <v>23</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1092,27 +1205,27 @@
         <v>24</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D27" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1120,13 +1233,13 @@
         <v>25</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D29" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1134,13 +1247,13 @@
         <v>26</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1148,20 +1261,20 @@
         <v>27</v>
       </c>
       <c r="C31" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D31" s="3" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
       <c r="B32" t="s">
         <v>28</v>
       </c>
-      <c r="C32" t="s">
+      <c r="C32" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1170,9 +1283,9 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>91</v>
-      </c>
-      <c r="C33" t="s">
+        <v>90</v>
+      </c>
+      <c r="C33" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1184,10 +1297,10 @@
         <v>30</v>
       </c>
       <c r="C34" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D34" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.3">
@@ -1198,10 +1311,10 @@
         <v>31</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D35" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.3">
@@ -1212,7 +1325,7 @@
         <v>32</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.3">
@@ -1223,10 +1336,10 @@
         <v>33</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.3">
@@ -1237,10 +1350,10 @@
         <v>34</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.3">
@@ -1251,7 +1364,7 @@
         <v>35</v>
       </c>
       <c r="C39" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.3">
@@ -1262,10 +1375,10 @@
         <v>36</v>
       </c>
       <c r="C40" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D40" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.3">
@@ -1276,10 +1389,10 @@
         <v>37</v>
       </c>
       <c r="C41" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D41" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.3">
@@ -1290,10 +1403,10 @@
         <v>38</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.3">
@@ -1301,13 +1414,13 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C43" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.3">
@@ -1318,10 +1431,10 @@
         <v>39</v>
       </c>
       <c r="C44" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D44" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.3">
@@ -1332,10 +1445,10 @@
         <v>40</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D45" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.3">
@@ -1345,7 +1458,7 @@
       <c r="B46" t="s">
         <v>41</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1357,10 +1470,10 @@
         <v>42</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.3">
@@ -1371,10 +1484,10 @@
         <v>43</v>
       </c>
       <c r="C48" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D48" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.3">
@@ -1385,10 +1498,10 @@
         <v>44</v>
       </c>
       <c r="C49" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.3">
@@ -1399,10 +1512,10 @@
         <v>45</v>
       </c>
       <c r="C50" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.3">
@@ -1413,10 +1526,10 @@
         <v>46</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.3">
@@ -1426,7 +1539,7 @@
       <c r="B52" t="s">
         <v>47</v>
       </c>
-      <c r="C52" t="s">
+      <c r="C52" s="2" t="s">
         <v>29</v>
       </c>
     </row>
@@ -1438,10 +1551,10 @@
         <v>48</v>
       </c>
       <c r="C53" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D53" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.3">
@@ -1452,7 +1565,7 @@
         <v>49</v>
       </c>
       <c r="C54" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.3">
@@ -1463,10 +1576,10 @@
         <v>50</v>
       </c>
       <c r="C55" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.3">
@@ -1477,10 +1590,10 @@
         <v>51</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.3">
@@ -1491,7 +1604,7 @@
         <v>52</v>
       </c>
       <c r="C57" s="3" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.3">
@@ -1526,7 +1639,7 @@
         <v>56</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.3">
@@ -1537,7 +1650,7 @@
         <v>57</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.3">
@@ -1548,7 +1661,7 @@
         <v>58</v>
       </c>
       <c r="C63" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.3">
@@ -1559,7 +1672,7 @@
         <v>59</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1569,8 +1682,8 @@
       <c r="B65" t="s">
         <v>60</v>
       </c>
-      <c r="C65" t="s">
-        <v>97</v>
+      <c r="C65" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
@@ -1580,8 +1693,8 @@
       <c r="B66" t="s">
         <v>61</v>
       </c>
-      <c r="C66" t="s">
-        <v>97</v>
+      <c r="C66" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
@@ -1591,8 +1704,8 @@
       <c r="B67" t="s">
         <v>62</v>
       </c>
-      <c r="C67" t="s">
-        <v>97</v>
+      <c r="C67" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
@@ -1602,8 +1715,8 @@
       <c r="B68" t="s">
         <v>63</v>
       </c>
-      <c r="C68" t="s">
-        <v>97</v>
+      <c r="C68" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
@@ -1613,7 +1726,7 @@
       <c r="B69" t="s">
         <v>64</v>
       </c>
-      <c r="C69" t="s">
+      <c r="C69" s="2" t="s">
         <v>66</v>
       </c>
     </row>
@@ -1622,10 +1735,10 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>102</v>
-      </c>
-      <c r="C70" t="s">
-        <v>97</v>
+        <v>101</v>
+      </c>
+      <c r="C70" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1635,8 +1748,8 @@
       <c r="B71" t="s">
         <v>65</v>
       </c>
-      <c r="C71" t="s">
-        <v>97</v>
+      <c r="C71" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
@@ -1646,8 +1759,8 @@
       <c r="B72" t="s">
         <v>67</v>
       </c>
-      <c r="C72" t="s">
-        <v>97</v>
+      <c r="C72" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1657,8 +1770,8 @@
       <c r="B73" t="s">
         <v>68</v>
       </c>
-      <c r="C73" t="s">
-        <v>97</v>
+      <c r="C73" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -1668,8 +1781,8 @@
       <c r="B74" t="s">
         <v>69</v>
       </c>
-      <c r="C74" t="s">
-        <v>97</v>
+      <c r="C74" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -1677,10 +1790,10 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>101</v>
-      </c>
-      <c r="C75" t="s">
-        <v>97</v>
+        <v>100</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -1690,8 +1803,8 @@
       <c r="B76" t="s">
         <v>70</v>
       </c>
-      <c r="C76" t="s">
-        <v>97</v>
+      <c r="C76" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -1699,13 +1812,13 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D77" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -1715,8 +1828,8 @@
       <c r="B78" t="s">
         <v>71</v>
       </c>
-      <c r="C78" t="s">
-        <v>97</v>
+      <c r="C78" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -1726,8 +1839,8 @@
       <c r="B79" t="s">
         <v>72</v>
       </c>
-      <c r="C79" t="s">
-        <v>97</v>
+      <c r="C79" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -1737,8 +1850,8 @@
       <c r="B80" t="s">
         <v>73</v>
       </c>
-      <c r="C80" t="s">
-        <v>97</v>
+      <c r="C80" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.3">
@@ -1748,8 +1861,8 @@
       <c r="B81" t="s">
         <v>74</v>
       </c>
-      <c r="C81" t="s">
-        <v>97</v>
+      <c r="C81" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.3">
@@ -1759,8 +1872,8 @@
       <c r="B82" t="s">
         <v>75</v>
       </c>
-      <c r="C82" t="s">
-        <v>97</v>
+      <c r="C82" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.3">
@@ -1770,8 +1883,8 @@
       <c r="B83" t="s">
         <v>76</v>
       </c>
-      <c r="C83" t="s">
-        <v>97</v>
+      <c r="C83" s="2" t="s">
+        <v>96</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.3">
@@ -1782,10 +1895,10 @@
         <v>77</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.3">
@@ -1796,7 +1909,7 @@
         <v>78</v>
       </c>
       <c r="C85" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.3">
@@ -1815,7 +1928,7 @@
         <v>80</v>
       </c>
       <c r="C87" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D87" s="4"/>
     </row>
@@ -1824,10 +1937,10 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C88" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D88" s="4"/>
     </row>
@@ -1839,7 +1952,7 @@
         <v>81</v>
       </c>
       <c r="C89" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D89" s="4"/>
     </row>
@@ -1848,10 +1961,10 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>82</v>
+        <v>105</v>
       </c>
       <c r="C90" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D90" s="4"/>
     </row>
@@ -1860,10 +1973,10 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C91" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D91" s="4"/>
     </row>
@@ -1872,10 +1985,10 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>92</v>
-      </c>
-      <c r="C92" t="s">
-        <v>97</v>
+        <v>91</v>
+      </c>
+      <c r="C92" s="2" t="s">
+        <v>96</v>
       </c>
       <c r="D92" s="4"/>
     </row>
@@ -1884,13 +1997,13 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C93" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D93" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.3">
@@ -1898,7 +2011,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
@@ -1908,13 +2021,13 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C95" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D95" s="4" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.3">
@@ -1922,10 +2035,26 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>98</v>
-      </c>
-      <c r="C96" t="s">
         <v>97</v>
+      </c>
+      <c r="C96" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97">
+        <v>96</v>
+      </c>
+      <c r="B97" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98">
+        <v>97</v>
+      </c>
+      <c r="B98" t="s">
+        <v>107</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Actualizacion 3 base de datos patrocinios
</commit_message>
<xml_diff>
--- a/Patrocinio/Base de datos patricinadores.xlsx
+++ b/Patrocinio/Base de datos patricinadores.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\entre\OneDrive\Desktop\FTC-Into_The_Deep\Patrocinio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\entre\Desktop\FTC-Into_The_Deep\Patrocinio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEF65441-5678-41D5-9B03-4DB43B9412B4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EF3060-75AB-418A-AE7C-28A589BD6E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BA4392A7-1F24-0648-8323-50C177A81C55}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="261" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="127">
   <si>
     <t xml:space="preserve">Juan Valdez </t>
   </si>
@@ -239,9 +239,6 @@
     <t xml:space="preserve">Primo Hurtado </t>
   </si>
   <si>
-    <t>Ryzen</t>
-  </si>
-  <si>
     <t>Intel</t>
   </si>
   <si>
@@ -314,9 +311,6 @@
     <t>Chocolatina JET</t>
   </si>
   <si>
-    <t>NO CONTACTADO</t>
-  </si>
-  <si>
     <t>#</t>
   </si>
   <si>
@@ -326,9 +320,6 @@
     <t>RESPUESTA</t>
   </si>
   <si>
-    <t xml:space="preserve">SIN CONTACTAR </t>
-  </si>
-  <si>
     <t>BOEING</t>
   </si>
   <si>
@@ -384,6 +375,48 @@
   </si>
   <si>
     <t>Esperando respuesta</t>
+  </si>
+  <si>
+    <t>Alfredo es retrasado y perdimos la propuesta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Llenar formulario para datos: https://co.asus.click/COLABORADORESASUS </t>
+  </si>
+  <si>
+    <t>AMD</t>
+  </si>
+  <si>
+    <t>Pepsico</t>
+  </si>
+  <si>
+    <t>Postobón</t>
+  </si>
+  <si>
+    <t>Rellenar formulario adjunto por el correo</t>
+  </si>
+  <si>
+    <t>Avianca</t>
+  </si>
+  <si>
+    <t>Enviar correo dirigido a Sergio González Villa al correo: serviciocliente@colanta.com</t>
+  </si>
+  <si>
+    <t>Hablar con Paola Suanca por el correo de los contactos</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
+  <si>
+    <t>Entendieron mal</t>
+  </si>
+  <si>
+    <t>No nos respondieron nada específico</t>
+  </si>
+  <si>
+    <t>Esperando respuesta (por Instagram)</t>
+  </si>
+  <si>
+    <t>Respuesta por correo, digeron que nos comunicáramos por otro lado (Instagram) y no nos han respondido</t>
   </si>
 </sst>
 </file>
@@ -467,7 +500,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - Tema de 2022">
   <a:themeElements>
     <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
@@ -763,40 +796,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{953E118B-2559-0648-84DD-D994D8679C8A}">
-  <dimension ref="A1:F98"/>
+  <dimension ref="A1:F101"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="20.296875" customWidth="1"/>
-    <col min="3" max="3" width="17" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" style="2" customWidth="1"/>
+    <col min="3" max="3" width="21.3984375" style="2" customWidth="1"/>
+    <col min="4" max="4" width="19.69921875" style="2" customWidth="1"/>
     <col min="5" max="5" width="25.09765625" style="2" customWidth="1"/>
-    <col min="6" max="6" width="58.69921875" style="2" customWidth="1"/>
+    <col min="6" max="6" width="94.09765625" style="2" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>86</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="E1" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>86</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>87</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>95</v>
-      </c>
       <c r="F1" s="5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
@@ -806,9 +839,6 @@
       <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>89</v>
-      </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3">
@@ -818,16 +848,16 @@
         <v>1</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F3" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
@@ -837,14 +867,14 @@
       <c r="B4" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="D4" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
@@ -855,13 +885,16 @@
         <v>3</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
@@ -871,14 +904,8 @@
       <c r="B6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="D6" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -889,13 +916,16 @@
         <v>5</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D7" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>29</v>
+        <v>88</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
@@ -906,13 +936,13 @@
         <v>6</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F8" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
@@ -923,13 +953,16 @@
         <v>7</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
@@ -940,13 +973,13 @@
         <v>8</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
@@ -957,13 +990,16 @@
         <v>9</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D11" s="2" t="s">
         <v>29</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>29</v>
+        <v>88</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
@@ -971,7 +1007,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -982,16 +1018,16 @@
         <v>10</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F13" s="2" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
@@ -1001,14 +1037,14 @@
       <c r="B14" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="D14" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
@@ -1018,14 +1054,14 @@
       <c r="B15" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="D15" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>109</v>
+        <v>88</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -1036,16 +1072,16 @@
         <v>13</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F16" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -1055,17 +1091,14 @@
       <c r="B17" t="s">
         <v>14</v>
       </c>
-      <c r="C17" s="2" t="s">
-        <v>89</v>
-      </c>
       <c r="D17" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F17" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
@@ -1075,11 +1108,9 @@
       <c r="B18" t="s">
         <v>15</v>
       </c>
-      <c r="C18" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C18" s="3"/>
       <c r="D18" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
@@ -1089,17 +1120,15 @@
       <c r="B19" t="s">
         <v>16</v>
       </c>
-      <c r="C19" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C19" s="3"/>
       <c r="D19" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="E19" s="2" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F19" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
@@ -1109,11 +1138,9 @@
       <c r="B20" t="s">
         <v>17</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C20" s="3"/>
       <c r="D20" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -1123,11 +1150,9 @@
       <c r="B21" t="s">
         <v>18</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C21" s="3"/>
       <c r="D21" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -1138,10 +1163,16 @@
         <v>19</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
@@ -1151,11 +1182,9 @@
       <c r="B23" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C23" s="3"/>
       <c r="D23" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -1165,8 +1194,9 @@
       <c r="B24" t="s">
         <v>21</v>
       </c>
-      <c r="C24" s="3" t="s">
-        <v>89</v>
+      <c r="C24" s="3"/>
+      <c r="D24" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
@@ -1176,11 +1206,15 @@
       <c r="B25" t="s">
         <v>22</v>
       </c>
-      <c r="C25" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C25" s="3"/>
       <c r="D25" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -1191,10 +1225,10 @@
         <v>23</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -1204,11 +1238,9 @@
       <c r="B27" t="s">
         <v>24</v>
       </c>
-      <c r="C27" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C27" s="3"/>
       <c r="D27" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
@@ -1216,13 +1248,19 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>113</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
@@ -1232,11 +1270,15 @@
       <c r="B29" t="s">
         <v>25</v>
       </c>
-      <c r="C29" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C29" s="3"/>
       <c r="D29" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
@@ -1247,10 +1289,10 @@
         <v>26</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>89</v>
+        <v>107</v>
       </c>
       <c r="D30" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
@@ -1260,11 +1302,9 @@
       <c r="B31" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C31" s="3"/>
       <c r="D31" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
@@ -1277,47 +1317,67 @@
       <c r="C32" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
       <c r="B34" t="s">
         <v>30</v>
       </c>
-      <c r="C34" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C34" s="3"/>
       <c r="D34" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
       <c r="B35" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C35" s="3"/>
       <c r="D35" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1325,24 +1385,37 @@
         <v>32</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
       <c r="B37" t="s">
         <v>33</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C37" s="3"/>
       <c r="D37" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1350,108 +1423,103 @@
         <v>34</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
       <c r="B39" t="s">
         <v>35</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C39" s="3"/>
+      <c r="D39" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
       <c r="B40" t="s">
         <v>36</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C40" s="3"/>
       <c r="D40" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
       <c r="B41" t="s">
         <v>37</v>
       </c>
-      <c r="C41" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C41" s="3"/>
       <c r="D41" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
       <c r="B42" t="s">
         <v>38</v>
       </c>
-      <c r="C42" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C42" s="3"/>
       <c r="D42" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>102</v>
-      </c>
-      <c r="C43" s="3" t="s">
-        <v>89</v>
-      </c>
+        <v>99</v>
+      </c>
+      <c r="C43" s="3"/>
       <c r="D43" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
       <c r="B44" t="s">
         <v>39</v>
       </c>
-      <c r="C44" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C44" s="3"/>
       <c r="D44" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
       <c r="B45" t="s">
         <v>40</v>
       </c>
-      <c r="C45" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C45" s="3"/>
       <c r="D45" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1461,8 +1529,17 @@
       <c r="C46" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D46" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E46" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F46" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1470,55 +1547,49 @@
         <v>42</v>
       </c>
       <c r="C47" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48">
         <v>47</v>
       </c>
       <c r="B48" t="s">
         <v>43</v>
       </c>
-      <c r="C48" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C48" s="3"/>
       <c r="D48" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49">
         <v>48</v>
       </c>
       <c r="B49" t="s">
         <v>44</v>
       </c>
-      <c r="C49" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C49" s="3"/>
       <c r="D49" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50">
         <v>49</v>
       </c>
       <c r="B50" t="s">
         <v>45</v>
       </c>
-      <c r="C50" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C50" s="3"/>
       <c r="D50" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1526,13 +1597,19 @@
         <v>46</v>
       </c>
       <c r="C51" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F51" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1542,47 +1619,53 @@
       <c r="C52" s="2" t="s">
         <v>29</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D52" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F52" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A53">
         <v>52</v>
       </c>
       <c r="B53" t="s">
         <v>48</v>
       </c>
-      <c r="C53" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C53" s="3"/>
       <c r="D53" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54">
         <v>53</v>
       </c>
       <c r="B54" t="s">
         <v>49</v>
       </c>
-      <c r="C54" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C54" s="3"/>
+      <c r="D54" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55">
         <v>54</v>
       </c>
       <c r="B55" t="s">
         <v>50</v>
       </c>
-      <c r="C55" s="3" t="s">
-        <v>89</v>
-      </c>
+      <c r="C55" s="3"/>
       <c r="D55" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1590,32 +1673,42 @@
         <v>51</v>
       </c>
       <c r="C56" s="3" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D56" s="3" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="E56" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57">
         <v>56</v>
       </c>
       <c r="B57" t="s">
         <v>52</v>
       </c>
-      <c r="C57" s="3" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C57" s="3"/>
+      <c r="D57" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58">
         <v>57</v>
       </c>
       <c r="B58" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="D58" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1623,7 +1716,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1631,7 +1724,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1639,10 +1732,16 @@
         <v>56</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="E61" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F61" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1650,21 +1749,25 @@
         <v>57</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="E62" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F62" s="2" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>62</v>
       </c>
       <c r="B63" t="s">
         <v>58</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="C63" s="4"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1672,7 +1775,13 @@
         <v>59</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
+      </c>
+      <c r="E64" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F64" s="2" t="s">
+        <v>105</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.3">
@@ -1682,9 +1791,6 @@
       <c r="B65" t="s">
         <v>60</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A66">
@@ -1693,9 +1799,6 @@
       <c r="B66" t="s">
         <v>61</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A67">
@@ -1704,9 +1807,6 @@
       <c r="B67" t="s">
         <v>62</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A68">
@@ -1715,9 +1815,6 @@
       <c r="B68" t="s">
         <v>63</v>
       </c>
-      <c r="C68" s="2" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A69">
@@ -1735,10 +1832,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>101</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.3">
@@ -1748,19 +1842,13 @@
       <c r="B71" t="s">
         <v>65</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>96</v>
-      </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A72">
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>67</v>
-      </c>
-      <c r="C72" s="2" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.3">
@@ -1768,10 +1856,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>68</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>96</v>
+        <v>67</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.3">
@@ -1779,10 +1864,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>69</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>96</v>
+        <v>68</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.3">
@@ -1790,10 +1872,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>100</v>
-      </c>
-      <c r="C75" s="2" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.3">
@@ -1801,10 +1880,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>70</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>96</v>
+        <v>69</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.3">
@@ -1812,13 +1888,11 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>99</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>96</v>
+      </c>
+      <c r="C77" s="4"/>
       <c r="D77" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.3">
@@ -1826,10 +1900,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>71</v>
-      </c>
-      <c r="C78" s="2" t="s">
-        <v>96</v>
+        <v>70</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.3">
@@ -1837,10 +1908,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>72</v>
-      </c>
-      <c r="C79" s="2" t="s">
-        <v>96</v>
+        <v>71</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.3">
@@ -1848,216 +1916,249 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>73</v>
-      </c>
-      <c r="C80" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81">
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>74</v>
-      </c>
-      <c r="C81" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82">
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>75</v>
-      </c>
-      <c r="C82" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83">
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>76</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.3">
+        <v>75</v>
+      </c>
+      <c r="D83" s="2" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84">
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C84" s="4" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D84" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+      <c r="E84" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F84" s="2" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85">
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>78</v>
-      </c>
-      <c r="C85" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+        <v>77</v>
+      </c>
+      <c r="C85" s="4"/>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>80</v>
-      </c>
-      <c r="C87" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D87" s="4"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+        <v>79</v>
+      </c>
+      <c r="C87" s="4"/>
+      <c r="D87" s="4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>98</v>
-      </c>
-      <c r="C88" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>95</v>
+      </c>
+      <c r="C88" s="4"/>
       <c r="D88" s="4"/>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>81</v>
-      </c>
-      <c r="C89" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>80</v>
+      </c>
+      <c r="C89" s="4"/>
       <c r="D89" s="4"/>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>105</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>102</v>
+      </c>
+      <c r="C90" s="4"/>
       <c r="D90" s="4"/>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>82</v>
-      </c>
-      <c r="C91" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>81</v>
+      </c>
+      <c r="C91" s="4"/>
       <c r="D91" s="4"/>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92">
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>91</v>
-      </c>
-      <c r="C92" s="2" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
       <c r="D92" s="4"/>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93">
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>83</v>
-      </c>
-      <c r="C93" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="D93" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+        <v>82</v>
+      </c>
+      <c r="C93" s="4"/>
+      <c r="D93" s="4"/>
+    </row>
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94">
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C94" s="4"/>
       <c r="D94" s="4"/>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A95">
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>85</v>
-      </c>
-      <c r="C95" s="4" t="s">
-        <v>89</v>
-      </c>
+        <v>84</v>
+      </c>
+      <c r="C95" s="4"/>
       <c r="D95" s="4" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96">
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>97</v>
-      </c>
-      <c r="C96" s="2" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97">
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+        <v>103</v>
+      </c>
+      <c r="C97" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="D97" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E97" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F97" s="2" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98">
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>107</v>
+        <v>104</v>
+      </c>
+      <c r="C98" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E98" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F98" s="2" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A99">
+        <v>98</v>
+      </c>
+      <c r="B99" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="100" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A100">
+        <v>99</v>
+      </c>
+      <c r="B100" t="s">
+        <v>117</v>
+      </c>
+      <c r="C100" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E100" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F100" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A101">
+        <v>100</v>
+      </c>
+      <c r="B101" t="s">
+        <v>119</v>
+      </c>
+      <c r="C101" s="2" t="s">
+        <v>88</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizacion 3.1 base de datos patrocinios
</commit_message>
<xml_diff>
--- a/Patrocinio/Base de datos patricinadores.xlsx
+++ b/Patrocinio/Base de datos patricinadores.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\entre\Desktop\FTC-Into_The_Deep\Patrocinio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EF3060-75AB-418A-AE7C-28A589BD6E67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47D52F2A-8BCA-4107-81BE-3ECCB0425C68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{BA4392A7-1F24-0648-8323-50C177A81C55}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="128">
   <si>
     <t xml:space="preserve">Juan Valdez </t>
   </si>
@@ -417,6 +417,9 @@
   </si>
   <si>
     <t>Respuesta por correo, digeron que nos comunicáramos por otro lado (Instagram) y no nos han respondido</t>
+  </si>
+  <si>
+    <t>Enviar correo a: patrocinios@avianca.com</t>
   </si>
 </sst>
 </file>
@@ -799,8 +802,8 @@
   <dimension ref="A1:F101"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B51" sqref="B51"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E80" sqref="E80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -2111,12 +2114,6 @@
       <c r="B98" t="s">
         <v>104</v>
       </c>
-      <c r="C98" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="E98" s="2" t="s">
-        <v>88</v>
-      </c>
       <c r="F98" s="2" t="s">
         <v>121</v>
       </c>
@@ -2153,8 +2150,14 @@
       <c r="B101" t="s">
         <v>119</v>
       </c>
-      <c r="C101" s="2" t="s">
-        <v>88</v>
+      <c r="D101" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="E101" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="F101" s="2" t="s">
+        <v>127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>